<commit_message>
FV6.pbit a FV6.pbix pridane s upravenými názvami stlpcov a s doplnenými udajmi o fakturácii
</commit_message>
<xml_diff>
--- a/FakturaciaSuhrn.xlsx
+++ b/FakturaciaSuhrn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MsDev\2020\Photovoltaics_Power_BI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F825363-64DA-4C14-80A9-A59DE38EBB6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A6295E-1549-4FFB-BCFD-E33ACAA29C29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{F0846DE4-5243-468C-B23C-E79FB8825FDF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{F0846DE4-5243-468C-B23C-E79FB8825FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Fakturácia" sheetId="1" r:id="rId1"/>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D123B9-3215-4493-95BB-D63BCC054DBD}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1559,45 +1559,24 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>12020</v>
-      </c>
       <c r="H28" s="4"/>
-      <c r="I28" s="6">
-        <f>SUBTOTAL(109,I2:I27)</f>
-        <v>1719.5324207260001</v>
-      </c>
-      <c r="J28" s="6">
-        <f>SUBTOTAL(109,J2:J27)</f>
-        <v>668.75282627999991</v>
-      </c>
-      <c r="K28" s="7">
-        <f>Table1[[#This Row],[Doplatok po rokoch]]+Table1[[#This Row],[Na straty po rokoch]]</f>
-        <v>2388.2852470059997</v>
-      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
-        <v>22020</v>
-      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
-        <v>12021</v>
-      </c>
       <c r="H30" s="4"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>22021</v>
-      </c>
       <c r="H31" s="4"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1622,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEFA5B55-B711-4851-95B5-BD9FDFFB723E}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>

</xml_diff>